<commit_message>
remove frank breitenbach from stakeholders
</commit_message>
<xml_diff>
--- a/Dokumente Projektinitiierung/Stakeholdermatrix.xlsx
+++ b/Dokumente Projektinitiierung/Stakeholdermatrix.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LuxLe\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leonlux/Developer/University/bachelorprojekt/Dokumente Projektinitiierung/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A29604C-45EB-4428-A874-ED618A2BED3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99F7A53D-5A54-B145-84EF-CEF1AC67EB75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38290" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{890167FE-D99A-408D-8CED-10CACF9CE310}"/>
+    <workbookView xWindow="4440" yWindow="760" windowWidth="25800" windowHeight="18880" xr2:uid="{890167FE-D99A-408D-8CED-10CACF9CE310}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
   <si>
     <t>Nr.</t>
   </si>
@@ -137,28 +137,6 @@
   </si>
   <si>
     <t>-</t>
-  </si>
-  <si>
-    <t>5.</t>
-  </si>
-  <si>
-    <t>Frank Breitenbach</t>
-  </si>
-  <si>
-    <t>Keine inhaltlichen Erwartungen (O)
-Sauberes Projektmanagement(O)
-Hoher Berichtoverhead(-)</t>
-  </si>
-  <si>
-    <t>Gar nicht</t>
-  </si>
-  <si>
-    <t>Inhatlich gar nicht, organisatorisch mittel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rücksprache bei Unsicherheiten
-Einhaltung von Termien
-</t>
   </si>
   <si>
     <t>Legende:</t>
@@ -292,9 +270,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-Design">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 – 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -332,7 +310,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 – 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -438,7 +416,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 – 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -580,7 +558,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -588,25 +566,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE1D5CC3-0C13-4071-B61D-59B0811C503D}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.90625" style="1"/>
-    <col min="2" max="2" width="18.36328125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.36328125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="25.90625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.36328125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.90625" style="1"/>
-    <col min="7" max="7" width="19.26953125" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.90625" style="1"/>
+    <col min="1" max="1" width="10.83203125" style="1"/>
+    <col min="2" max="2" width="18.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="25.83203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="1"/>
+    <col min="7" max="7" width="19.33203125" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -629,7 +607,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="144" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -652,7 +630,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="145" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" ht="144" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -675,7 +653,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="188.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" ht="208" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>16</v>
       </c>
@@ -698,7 +676,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" ht="80" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>24</v>
       </c>
@@ -721,40 +699,17 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="5" t="s">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B7" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="6" t="s">
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B8" s="10" t="s">
         <v>31</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B9" s="10" t="s">
-        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>